<commit_message>
Updates for gold demand and price averaging
- added historical_price_rolling_window as an input for the Sensitivity class, allows taking the moving average (centered) over however-many years given, default 1
- added rmse_df to the things saved in big_df and as a result, saved in the big pickle file, since there appears to be inconsistency between those values and the values in the indiv.hyperparam df
- added moving average capability to the gold demand volume drivers, and updated the previous coins/bullion volume driver to be from World Bank, global cash reserves in gold bullion rather than US circulating coin production
- changed the way volumes are adjusted to match the volume_growth_rate input parameter, since there was something funky there
</commit_message>
<xml_diff>
--- a/data/Gold demand volume indicators.xlsx
+++ b/data/Gold demand volume indicators.xlsx
@@ -8,15 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ryter\Dropbox (MIT)\John MIT\Research\generalizationOutside\generalization\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C8C73C0-4C0D-430B-B5EC-1E8C8DB4D48A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B1B925F-4186-480A-80F9-7E4FF4C9FF04}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="456" windowWidth="23040" windowHeight="8904" xr2:uid="{9A215CAF-1FA5-4765-BCEC-C58550B88C4B}"/>
+    <workbookView xWindow="0" yWindow="912" windowWidth="23040" windowHeight="8904" xr2:uid="{9A215CAF-1FA5-4765-BCEC-C58550B88C4B}"/>
   </bookViews>
   <sheets>
     <sheet name="Volume drivers" sheetId="1" r:id="rId1"/>
     <sheet name="Sectoral demand" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
+    <definedName name="factor">'Volume drivers'!$C$7</definedName>
     <definedName name="IQ_CH">110000</definedName>
     <definedName name="IQ_CQ">5000</definedName>
     <definedName name="IQ_CY">10000</definedName>
@@ -54,7 +55,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
   <si>
     <t>American Buffalo Gold Bullion (oz)</t>
   </si>
@@ -81,6 +82,12 @@
   </si>
   <si>
     <t>Bain Diamond Report 2020-21 p52 https://www.bain.com/globalassets/noindex/2021/bain_report_diamond_report-2020-21.pdf, could be used to represent jewelry demand, made assumptions about the longer-term future based on the projections given in the report</t>
+  </si>
+  <si>
+    <t>Global gold cash reserves (USD$2021)</t>
+  </si>
+  <si>
+    <t>From the World Bank, using two data series: [Total reserves (includes gold, current US$)] and [Total reserves minus gold (current US$)]. Accessed here: https://data.worldbank.org/indicator?tab=all, excel files were downloaded and the total minus gold was subtracted from total including gold.For 2022 onward, assumed constant slope, same as average 2016-2021</t>
   </si>
 </sst>
 </file>
@@ -944,6 +951,741 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>American Buffalo Bullion</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>'Volume drivers'!$B$3:$B$22</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="20"/>
+                <c:pt idx="0">
+                  <c:v>237434.68067187499</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>249931.24281249999</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>263085.51874999999</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>276932.125</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>291507.5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>306850</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>323000</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>167500</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>172000</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>200000</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>209000</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>174500</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>132000</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>239000</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>177500</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>220500</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>219500</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>99500</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>121500</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>61500</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-6219-460E-9591-8A3114BAAA11}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:smooth val="0"/>
+        <c:axId val="716191336"/>
+        <c:axId val="716185432"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="716191336"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="716185432"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="716185432"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="716191336"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Global gold reserves (World Bank)</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>'Volume drivers'!$F$3:$F$43</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="41"/>
+                <c:pt idx="0">
+                  <c:v>2454657984118.7334</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2556294563744.75</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2987402776563.8701</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3636797568319.9302</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>4321596159618.8315</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>4879605854471.252</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>5936101889017.9287</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>7612829279727.3828</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>8276433678396.0869</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>9684483542285.0078</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>10897602055805.906</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>12323478668659.906</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>13253175023758.746</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>13441269212269.359</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>13311505925855.328</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>12442558668238.301</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>12325176119458.914</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>13249242685825.994</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>13243791725100.152</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>13964690030137.049</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>15291304937082.742</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>15987064622366.021</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>16577815614720.641</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>17168566607075.262</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>17759317599429.883</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>18350068591784.504</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>18940819584139.125</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>19531570576493.746</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>20122321568848.367</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>20713072561202.988</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>21303823553557.609</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>21894574545912.23</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>22485325538266.852</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>23076076530621.473</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>23666827522976.094</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>24257578515330.715</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>24848329507685.336</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>25439080500039.957</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>26029831492394.578</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>26620582484749.199</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>27211333477103.82</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-9F3E-40A6-8C6B-3FCF1321687A}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:smooth val="0"/>
+        <c:axId val="990516640"/>
+        <c:axId val="990515328"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="990516640"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="990515328"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="990515328"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="990516640"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
@@ -1024,6 +1766,86 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors4.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
   <cs:axisTitle>
@@ -2056,20 +2878,1052 @@
 </cs:chartStyle>
 </file>
 
+<file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style4.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>259080</xdr:colOff>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>99060</xdr:colOff>
       <xdr:row>1</xdr:row>
-      <xdr:rowOff>148590</xdr:rowOff>
+      <xdr:rowOff>156210</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>563880</xdr:colOff>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>403860</xdr:colOff>
       <xdr:row>17</xdr:row>
-      <xdr:rowOff>148590</xdr:rowOff>
+      <xdr:rowOff>156210</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -2096,16 +3950,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>251460</xdr:colOff>
-      <xdr:row>18</xdr:row>
-      <xdr:rowOff>102870</xdr:rowOff>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>259080</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>49530</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>556260</xdr:colOff>
-      <xdr:row>33</xdr:row>
-      <xdr:rowOff>102870</xdr:rowOff>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>563880</xdr:colOff>
+      <xdr:row>36</xdr:row>
+      <xdr:rowOff>49530</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -2125,6 +3979,78 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>76200</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>381000</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E35D4209-1AFB-42EE-B416-1D11B70EC304}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>60960</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>49530</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>365760</xdr:colOff>
+      <xdr:row>36</xdr:row>
+      <xdr:rowOff>49530</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="5" name="Chart 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5A0CA486-EC5A-4A67-8683-2BE3824B3556}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId4"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -2430,15 +4356,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F0C59811-5519-45BC-9A7C-7F8C67C8D8FA}">
-  <dimension ref="A1:E43"/>
+  <dimension ref="A1:H43"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
+      <selection activeCell="G32" sqref="G32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="6" max="6" width="12" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B1" t="s">
         <v>0</v>
       </c>
@@ -2451,8 +4381,11 @@
       <c r="E1" t="s">
         <v>6</v>
       </c>
+      <c r="F1" t="s">
+        <v>9</v>
+      </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -2468,75 +4401,122 @@
       <c r="E2" t="s">
         <v>8</v>
       </c>
+      <c r="F2" t="s">
+        <v>10</v>
+      </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>2000</v>
       </c>
-      <c r="B3" s="1"/>
+      <c r="B3">
+        <f>B4*factor</f>
+        <v>237434.68067187499</v>
+      </c>
       <c r="D3">
         <v>27100</v>
       </c>
       <c r="E3">
         <v>9.75</v>
       </c>
+      <c r="F3">
+        <v>2454657984118.7334</v>
+      </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>2001</v>
       </c>
+      <c r="B4">
+        <f>B5*factor</f>
+        <v>249931.24281249999</v>
+      </c>
       <c r="D4">
         <v>23530.658990853801</v>
       </c>
       <c r="E4">
         <v>9.4563106796116294</v>
       </c>
+      <c r="F4">
+        <v>2556294563744.75</v>
+      </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>2002</v>
       </c>
+      <c r="B5">
+        <f>B6*factor</f>
+        <v>263085.51874999999</v>
+      </c>
       <c r="D5">
         <v>14862.472296514599</v>
       </c>
       <c r="E5">
         <v>10.1844660194174</v>
       </c>
+      <c r="F5">
+        <v>2987402776563.8701</v>
+      </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>2003</v>
       </c>
+      <c r="B6">
+        <f>B7*factor</f>
+        <v>276932.125</v>
+      </c>
       <c r="D6">
         <v>11222.2185630693</v>
       </c>
       <c r="E6">
         <v>11.0145631067961</v>
       </c>
+      <c r="F6">
+        <v>3636797568319.9302</v>
+      </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>2004</v>
       </c>
+      <c r="B7">
+        <f>B8*factor</f>
+        <v>291507.5</v>
+      </c>
+      <c r="C7">
+        <v>0.95</v>
+      </c>
       <c r="D7">
         <v>13376.0800242718</v>
       </c>
       <c r="E7">
         <v>11.2330097087378</v>
       </c>
+      <c r="F7">
+        <v>4321596159618.8315</v>
+      </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>2005</v>
       </c>
+      <c r="B8">
+        <f>B9*factor</f>
+        <v>306850</v>
+      </c>
       <c r="D8">
         <v>14165.2588659911</v>
       </c>
       <c r="E8">
         <v>12.4126213592232</v>
       </c>
+      <c r="F8">
+        <v>4879605854471.252</v>
+      </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>2006</v>
       </c>
@@ -2549,8 +4529,11 @@
       <c r="E9">
         <v>12.791262135922301</v>
       </c>
+      <c r="F9">
+        <v>5936101889017.9287</v>
+      </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>2007</v>
       </c>
@@ -2563,8 +4546,11 @@
       <c r="E10">
         <v>13.1844660194174</v>
       </c>
+      <c r="F10">
+        <v>7612829279727.3828</v>
+      </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>2008</v>
       </c>
@@ -2577,8 +4563,11 @@
       <c r="E11">
         <v>13.1844660194174</v>
       </c>
+      <c r="F11">
+        <v>8276433678396.0869</v>
+      </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>2009</v>
       </c>
@@ -2591,8 +4580,11 @@
       <c r="E12">
         <v>8.8883495145629894</v>
       </c>
+      <c r="F12">
+        <v>9684483542285.0078</v>
+      </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>2010</v>
       </c>
@@ -2605,8 +4597,11 @@
       <c r="E13">
         <v>12.063106796116401</v>
       </c>
+      <c r="F13">
+        <v>10897602055805.906</v>
+      </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>2011</v>
       </c>
@@ -2619,8 +4614,11 @@
       <c r="E14">
         <v>14.364077669902899</v>
       </c>
+      <c r="F14">
+        <v>12323478668659.906</v>
+      </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>2012</v>
       </c>
@@ -2636,8 +4634,15 @@
       <c r="E15">
         <v>13.7961165048543</v>
       </c>
+      <c r="F15">
+        <v>13253175023758.746</v>
+      </c>
+      <c r="G15">
+        <f t="shared" ref="G15:G17" si="0">F15/F14</f>
+        <v>1.075441064986234</v>
+      </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>2013</v>
       </c>
@@ -2653,8 +4658,15 @@
       <c r="E16">
         <v>14.4514563106796</v>
       </c>
+      <c r="F16">
+        <v>13441269212269.359</v>
+      </c>
+      <c r="G16">
+        <f t="shared" si="0"/>
+        <v>1.0141923869694183</v>
+      </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>2014</v>
       </c>
@@ -2670,8 +4682,15 @@
       <c r="E17">
         <v>16.723300970873701</v>
       </c>
+      <c r="F17">
+        <v>13311505925855.328</v>
+      </c>
+      <c r="G17">
+        <f t="shared" si="0"/>
+        <v>0.99034590525903743</v>
+      </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>2015</v>
       </c>
@@ -2687,8 +4706,15 @@
       <c r="E18">
         <v>11.917475728155299</v>
       </c>
+      <c r="F18">
+        <v>12442558668238.301</v>
+      </c>
+      <c r="G18">
+        <f>F18/F17</f>
+        <v>0.93472209211662183</v>
+      </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>2016</v>
       </c>
@@ -2704,8 +4730,19 @@
       <c r="E19">
         <v>14.1893203883495</v>
       </c>
+      <c r="F19">
+        <v>12325176119458.914</v>
+      </c>
+      <c r="G19">
+        <f t="shared" ref="G19:G23" si="1">F19/F18</f>
+        <v>0.99056604417875682</v>
+      </c>
+      <c r="H19">
+        <f t="shared" ref="H19:H23" si="2">F19-F18</f>
+        <v>-117382548779.38672</v>
+      </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>2017</v>
       </c>
@@ -2721,8 +4758,19 @@
       <c r="E20">
         <v>14.597087378640699</v>
       </c>
+      <c r="F20">
+        <v>13249242685825.994</v>
+      </c>
+      <c r="G20">
+        <f t="shared" si="1"/>
+        <v>1.0749739036108514</v>
+      </c>
+      <c r="H20">
+        <f t="shared" si="2"/>
+        <v>924066566367.08008</v>
+      </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>2018</v>
       </c>
@@ -2738,8 +4786,19 @@
       <c r="E21">
         <v>15.135922330096999</v>
       </c>
+      <c r="F21">
+        <v>13243791725100.152</v>
+      </c>
+      <c r="G21">
+        <f t="shared" si="1"/>
+        <v>0.99958858322282274</v>
+      </c>
+      <c r="H21">
+        <f t="shared" si="2"/>
+        <v>-5450960725.8417969</v>
+      </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>2019</v>
       </c>
@@ -2755,8 +4814,19 @@
       <c r="E22">
         <v>12.4271844660194</v>
       </c>
+      <c r="F22">
+        <v>13964690030137.049</v>
+      </c>
+      <c r="G22">
+        <f t="shared" si="1"/>
+        <v>1.0544329237427241</v>
+      </c>
+      <c r="H22">
+        <f t="shared" si="2"/>
+        <v>720898305036.89648</v>
+      </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A23">
         <v>2020</v>
       </c>
@@ -2769,8 +4839,19 @@
       <c r="E23">
         <v>8.2038834951456092</v>
       </c>
+      <c r="F23">
+        <v>15291304937082.742</v>
+      </c>
+      <c r="G23">
+        <f t="shared" si="1"/>
+        <v>1.0949978054709943</v>
+      </c>
+      <c r="H23">
+        <f t="shared" si="2"/>
+        <v>1326614906945.6934</v>
+      </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A24">
         <v>2021</v>
       </c>
@@ -2784,8 +4865,19 @@
         <f>E23*1.3</f>
         <v>10.665048543689293</v>
       </c>
+      <c r="F24">
+        <v>15987064622366.021</v>
+      </c>
+      <c r="G24">
+        <f>F24/F23</f>
+        <v>1.0455003472984181</v>
+      </c>
+      <c r="H24">
+        <f>F24-F23</f>
+        <v>695759685283.2793</v>
+      </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A25">
         <v>2022</v>
       </c>
@@ -2797,239 +4889,323 @@
         <f>E24*1.15</f>
         <v>12.264805825242686</v>
       </c>
+      <c r="F25">
+        <f>F24+$H$26</f>
+        <v>16577815614720.641</v>
+      </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A26">
         <v>2023</v>
       </c>
       <c r="D26">
-        <f t="shared" ref="D26:D43" si="0">D25*1.01</f>
+        <f t="shared" ref="D26:D43" si="3">D25*1.01</f>
         <v>14946.904840848943</v>
       </c>
       <c r="E26">
         <f>E25*1.02</f>
         <v>12.510101941747539</v>
       </c>
+      <c r="F26">
+        <f t="shared" ref="F26:F43" si="4">F25+$H$26</f>
+        <v>17168566607075.262</v>
+      </c>
+      <c r="G26">
+        <f>AVERAGE(G19:G24)</f>
+        <v>1.0433432679207613</v>
+      </c>
+      <c r="H26">
+        <f>AVERAGE(H19:H24)</f>
+        <v>590750992354.62012</v>
+      </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A27">
         <v>2024</v>
       </c>
       <c r="D27">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>15096.373889257433</v>
       </c>
       <c r="E27">
         <f>E26*1.015</f>
         <v>12.697753470873751</v>
       </c>
+      <c r="F27">
+        <f t="shared" si="4"/>
+        <v>17759317599429.883</v>
+      </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A28">
         <v>2025</v>
       </c>
       <c r="D28">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>15247.337628150008</v>
       </c>
       <c r="E28">
-        <f t="shared" ref="E28:E43" si="1">E27*1.015</f>
+        <f t="shared" ref="E28:E43" si="5">E27*1.015</f>
         <v>12.888219772936857</v>
       </c>
+      <c r="F28">
+        <f t="shared" si="4"/>
+        <v>18350068591784.504</v>
+      </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A29">
         <v>2026</v>
       </c>
       <c r="D29">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>15399.811004431507</v>
       </c>
       <c r="E29">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>13.081543069530909</v>
       </c>
+      <c r="F29">
+        <f t="shared" si="4"/>
+        <v>18940819584139.125</v>
+      </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A30">
         <v>2027</v>
       </c>
       <c r="D30">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>15553.809114475822</v>
       </c>
       <c r="E30">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>13.277766215573871</v>
       </c>
+      <c r="F30">
+        <f t="shared" si="4"/>
+        <v>19531570576493.746</v>
+      </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A31">
         <v>2028</v>
       </c>
       <c r="D31">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>15709.347205620581</v>
       </c>
       <c r="E31">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>13.476932708807478</v>
       </c>
+      <c r="F31">
+        <f t="shared" si="4"/>
+        <v>20122321568848.367</v>
+      </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A32">
         <v>2029</v>
       </c>
       <c r="D32">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>15866.440677676786</v>
       </c>
       <c r="E32">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>13.679086699439589</v>
       </c>
+      <c r="F32">
+        <f t="shared" si="4"/>
+        <v>20713072561202.988</v>
+      </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A33">
         <v>2030</v>
       </c>
       <c r="D33">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>16025.105084453555</v>
       </c>
       <c r="E33">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>13.884272999931181</v>
       </c>
+      <c r="F33">
+        <f t="shared" si="4"/>
+        <v>21303823553557.609</v>
+      </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A34">
         <v>2031</v>
       </c>
       <c r="D34">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>16185.356135298091</v>
       </c>
       <c r="E34">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>14.092537094930147</v>
       </c>
+      <c r="F34">
+        <f t="shared" si="4"/>
+        <v>21894574545912.23</v>
+      </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A35">
         <v>2032</v>
       </c>
       <c r="D35">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>16347.209696651071</v>
       </c>
       <c r="E35">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>14.303925151354099</v>
       </c>
+      <c r="F35">
+        <f t="shared" si="4"/>
+        <v>22485325538266.852</v>
+      </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A36">
         <v>2033</v>
       </c>
       <c r="D36">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>16510.681793617583</v>
       </c>
       <c r="E36">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>14.518484028624409</v>
       </c>
+      <c r="F36">
+        <f t="shared" si="4"/>
+        <v>23076076530621.473</v>
+      </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A37">
         <v>2034</v>
       </c>
       <c r="D37">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>16675.788611553759</v>
       </c>
       <c r="E37">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>14.736261289053774</v>
       </c>
+      <c r="F37">
+        <f t="shared" si="4"/>
+        <v>23666827522976.094</v>
+      </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A38">
         <v>2035</v>
       </c>
       <c r="D38">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>16842.546497669297</v>
       </c>
       <c r="E38">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>14.957305208389579</v>
       </c>
+      <c r="F38">
+        <f t="shared" si="4"/>
+        <v>24257578515330.715</v>
+      </c>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A39">
         <v>2036</v>
       </c>
       <c r="D39">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>17010.971962645988</v>
       </c>
       <c r="E39">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>15.181664786515421</v>
       </c>
+      <c r="F39">
+        <f t="shared" si="4"/>
+        <v>24848329507685.336</v>
+      </c>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A40">
         <v>2037</v>
       </c>
       <c r="D40">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>17181.081682272448</v>
       </c>
       <c r="E40">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>15.409389758313152</v>
       </c>
+      <c r="F40">
+        <f t="shared" si="4"/>
+        <v>25439080500039.957</v>
+      </c>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A41">
         <v>2038</v>
       </c>
       <c r="D41">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>17352.892499095175</v>
       </c>
       <c r="E41">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>15.640530604687848</v>
       </c>
+      <c r="F41">
+        <f t="shared" si="4"/>
+        <v>26029831492394.578</v>
+      </c>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A42">
         <v>2039</v>
       </c>
       <c r="D42">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>17526.421424086126</v>
       </c>
       <c r="E42">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>15.875138563758165</v>
       </c>
+      <c r="F42">
+        <f t="shared" si="4"/>
+        <v>26620582484749.199</v>
+      </c>
     </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A43">
         <v>2040</v>
       </c>
       <c r="D43">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>17701.685638326988</v>
       </c>
       <c r="E43">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>16.113265642214536</v>
+      </c>
+      <c r="F43">
+        <f t="shared" si="4"/>
+        <v>27211333477103.82</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updating notes and title for gold volume driver
Was using cash reserves all along, rather than the gold-only version of cash reserves
</commit_message>
<xml_diff>
--- a/data/Gold demand volume indicators.xlsx
+++ b/data/Gold demand volume indicators.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ryter\Dropbox (MIT)\John MIT\Research\generalizationOutside\generalization\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B1B925F-4186-480A-80F9-7E4FF4C9FF04}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6DD4B137-6647-40BA-8113-1E448B1BAB83}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="912" windowWidth="23040" windowHeight="8904" xr2:uid="{9A215CAF-1FA5-4765-BCEC-C58550B88C4B}"/>
   </bookViews>
@@ -84,10 +84,10 @@
     <t>Bain Diamond Report 2020-21 p52 https://www.bain.com/globalassets/noindex/2021/bain_report_diamond_report-2020-21.pdf, could be used to represent jewelry demand, made assumptions about the longer-term future based on the projections given in the report</t>
   </si>
   <si>
-    <t>Global gold cash reserves (USD$2021)</t>
+    <t>From the World Bank, using two data series: [Total reserves (includes gold, current US$)] and [Total reserves minus gold (current US$)]. Accessed here: https://data.worldbank.org/indicator?tab=all, excel files were downloaded and the total minus gold was subtracted from total including gold.For 2022 onward, assumed constant slope, same as average 2016-2021</t>
   </si>
   <si>
-    <t>From the World Bank, using two data series: [Total reserves (includes gold, current US$)] and [Total reserves minus gold (current US$)]. Accessed here: https://data.worldbank.org/indicator?tab=all, excel files were downloaded and the total minus gold was subtracted from total including gold.For 2022 onward, assumed constant slope, same as average 2016-2021</t>
+    <t>Global cash reserves (USD$2021)</t>
   </si>
 </sst>
 </file>
@@ -4358,8 +4358,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F0C59811-5519-45BC-9A7C-7F8C67C8D8FA}">
   <dimension ref="A1:H43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
-      <selection activeCell="G32" sqref="G32"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4382,7 +4382,7 @@
         <v>6</v>
       </c>
       <c r="F1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
@@ -4402,7 +4402,7 @@
         <v>8</v>
       </c>
       <c r="F2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Update Gold demand volume indicators.xlsx
unsure if this is any different from the last commit but didn't want to risk it
</commit_message>
<xml_diff>
--- a/data/Gold demand volume indicators.xlsx
+++ b/data/Gold demand volume indicators.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ryter\Dropbox (MIT)\John MIT\Research\generalizationOutside\generalization\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6DD4B137-6647-40BA-8113-1E448B1BAB83}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{148C1B22-4FA2-46A4-9BC5-66D5E155F8F3}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="912" windowWidth="23040" windowHeight="8904" xr2:uid="{9A215CAF-1FA5-4765-BCEC-C58550B88C4B}"/>
   </bookViews>
@@ -84,10 +84,10 @@
     <t>Bain Diamond Report 2020-21 p52 https://www.bain.com/globalassets/noindex/2021/bain_report_diamond_report-2020-21.pdf, could be used to represent jewelry demand, made assumptions about the longer-term future based on the projections given in the report</t>
   </si>
   <si>
-    <t>From the World Bank, using two data series: [Total reserves (includes gold, current US$)] and [Total reserves minus gold (current US$)]. Accessed here: https://data.worldbank.org/indicator?tab=all, excel files were downloaded and the total minus gold was subtracted from total including gold.For 2022 onward, assumed constant slope, same as average 2016-2021</t>
+    <t>Global cash reserves (USD$2021)</t>
   </si>
   <si>
-    <t>Global cash reserves (USD$2021)</t>
+    <t>From the World Bank, using data series: [Total reserves (includes gold, current US$)]. Accessed here: https://data.worldbank.org/indicator?tab=all, excel files were downloaded.For 2022 onward, assumed constant slope, same as average 2016-2021</t>
   </si>
 </sst>
 </file>
@@ -4359,7 +4359,7 @@
   <dimension ref="A1:H43"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4382,7 +4382,7 @@
         <v>6</v>
       </c>
       <c r="F1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
@@ -4402,7 +4402,7 @@
         <v>8</v>
       </c>
       <c r="F2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">

</xml_diff>